<commit_message>
zaw - DB Design Initial Commit
</commit_message>
<xml_diff>
--- a/documentation/01_DB設計/01_テーブル一覧.xlsx
+++ b/documentation/01_DB設計/01_テーブル一覧.xlsx
@@ -58,7 +58,7 @@
     <t>本管理するため使用</t>
   </si>
   <si>
-    <t>ゾーレ</t>
+    <t>ゾー</t>
   </si>
   <si>
     <t>user</t>
@@ -73,28 +73,28 @@
     <t>user_shipping</t>
   </si>
   <si>
-    <t>ユーザーの配送データ</t>
-  </si>
-  <si>
-    <t>ユーザーの配送データを管理するため使用</t>
+    <t>ユーザー配送データ</t>
+  </si>
+  <si>
+    <t>ユーザー配送データを管理するため使用</t>
   </si>
   <si>
     <t>user_billing</t>
   </si>
   <si>
-    <t>ユーザーの請求データ</t>
-  </si>
-  <si>
-    <t>ユーザーの請求データを管理するため使用</t>
+    <t>ユーザー請求データ</t>
+  </si>
+  <si>
+    <t>ユーザー請求データを管理するため使用</t>
   </si>
   <si>
     <t>user_payment</t>
   </si>
   <si>
-    <t>ユーザーの支払いデータ</t>
-  </si>
-  <si>
-    <t>ユーザーの支払いデータを管理するため使用</t>
+    <t>ユーザー支払いデータ</t>
+  </si>
+  <si>
+    <t>ユーザー支払いデータを管理するため使用</t>
   </si>
   <si>
     <t>cart_item</t>
@@ -142,10 +142,10 @@
     <t>支払いを保持するため使用</t>
   </si>
   <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>注文データ</t>
+    <t>user_order</t>
+  </si>
+  <si>
+    <t>ユーザー注文データ</t>
   </si>
   <si>
     <t>注文データを保持するため使用</t>
@@ -156,12 +156,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +176,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -185,60 +208,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,25 +253,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -282,6 +276,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -299,14 +307,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,23 +326,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,19 +348,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,163 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,21 +541,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,6 +569,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -623,6 +604,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,167 +642,156 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -831,7 +812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,7 +1139,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78095238095238" defaultRowHeight="15"/>
@@ -1293,13 +1273,13 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1308,9 +1288,9 @@
       <c r="G6" s="8">
         <v>44902</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="9">
@@ -1319,13 +1299,13 @@
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1334,9 +1314,9 @@
       <c r="G7" s="8">
         <v>44902</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="9">
@@ -1345,13 +1325,13 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1360,9 +1340,9 @@
       <c r="G8" s="8">
         <v>44902</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="9">
@@ -1371,13 +1351,13 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1386,9 +1366,9 @@
       <c r="G9" s="8">
         <v>44902</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="9">
@@ -1397,13 +1377,13 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1412,9 +1392,9 @@
       <c r="G10" s="8">
         <v>44902</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="9">
@@ -1423,13 +1403,13 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1438,9 +1418,9 @@
       <c r="G11" s="8">
         <v>44902</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="9">
@@ -1449,13 +1429,13 @@
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1464,9 +1444,9 @@
       <c r="G12" s="8">
         <v>44902</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="9">
@@ -1475,13 +1455,13 @@
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1490,9 +1470,9 @@
       <c r="G13" s="8">
         <v>44902</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>